<commit_message>
Mouser part numbers update
</commit_message>
<xml_diff>
--- a/1uO_c_2.2_BOM.xlsx
+++ b/1uO_c_2.2_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shayshez/Documents/eagle/projects/1uO_c/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shayshez/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78A5943-AAC8-1E43-BEAB-89C3DAB53A39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006F37F5-0C79-1C4A-9247-60105CCA88EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="20540" xr2:uid="{294FFD5C-7B87-654B-82DB-03171BED3865}"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21140" xr2:uid="{294FFD5C-7B87-654B-82DB-03171BED3865}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{2BA751CE-CDD5-6343-94D5-EF8248ABB28E}" name="1uO_c_v_2.2" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/shayshez/Documents/eagle/projects/1uO_c/1uO_c_v_2.2.csv" tab="0" semicolon="1">
+    <textPr sourceFile="/Users/shayshez/Documents/eagle/projects/1uO_c/1uO_c_v_2.2.csv" tab="0" semicolon="1">
       <textFields count="24">
         <textField/>
         <textField/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="213">
   <si>
     <t>Qty</t>
   </si>
@@ -638,21 +638,9 @@
     <t>603-RC0603FR-07510RL</t>
   </si>
   <si>
-    <t>603-RC0603FR-102KL</t>
-  </si>
-  <si>
-    <t>603-RC0603FR-0710KL</t>
-  </si>
-  <si>
-    <t>603-RC0603FR-0724K9L</t>
-  </si>
-  <si>
     <t>603-RC0603FR-1333KL</t>
   </si>
   <si>
-    <t>603-RC0603FR-0747KL</t>
-  </si>
-  <si>
     <t>603-AC0603FR-0775KL</t>
   </si>
   <si>
@@ -683,9 +671,6 @@
     <t>667-EEE-FK1H220SR</t>
   </si>
   <si>
-    <t>963-LMK107BBJ106KALT</t>
-  </si>
-  <si>
     <t>647-UWX1C100MCL2</t>
   </si>
   <si>
@@ -753,6 +738,18 @@
   </si>
   <si>
     <t>https://github.com/Shayshez/1_3_OLED_FOR_1U</t>
+  </si>
+  <si>
+    <t>603-RC0603FR-072KL</t>
+  </si>
+  <si>
+    <t>603-AC0603FR-1010KL</t>
+  </si>
+  <si>
+    <t>603-RC0603FR-0724KL</t>
+  </si>
+  <si>
+    <t>810-C1608X5R1A106K</t>
   </si>
 </sst>
 </file>
@@ -1192,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C8E2A90-1924-FD4B-A7BC-73636687E665}">
   <dimension ref="A1:W48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1298,9 +1295,6 @@
       <c r="B2" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="G2" t="s">
-        <v>172</v>
-      </c>
     </row>
     <row r="3" spans="1:23">
       <c r="A3">
@@ -1322,7 +1316,7 @@
         <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="U3" t="s">
         <v>28</v>
@@ -1348,7 +1342,7 @@
         <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="U4" t="s">
         <v>28</v>
@@ -1374,7 +1368,7 @@
         <v>27</v>
       </c>
       <c r="G5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U5" t="s">
         <v>28</v>
@@ -1400,7 +1394,7 @@
         <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>176</v>
+        <v>209</v>
       </c>
       <c r="U6" t="s">
         <v>28</v>
@@ -1426,7 +1420,7 @@
         <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>177</v>
+        <v>210</v>
       </c>
       <c r="U7" t="s">
         <v>28</v>
@@ -1452,7 +1446,7 @@
         <v>27</v>
       </c>
       <c r="G8" t="s">
-        <v>178</v>
+        <v>211</v>
       </c>
       <c r="U8" t="s">
         <v>28</v>
@@ -1478,7 +1472,7 @@
         <v>27</v>
       </c>
       <c r="G9" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="U9" t="s">
         <v>28</v>
@@ -1504,7 +1498,7 @@
         <v>27</v>
       </c>
       <c r="G10" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="U10" t="s">
         <v>28</v>
@@ -1530,7 +1524,7 @@
         <v>27</v>
       </c>
       <c r="G11" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="U11" t="s">
         <v>28</v>
@@ -1561,7 +1555,7 @@
         <v>35</v>
       </c>
       <c r="G13" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:23">
@@ -1584,7 +1578,7 @@
         <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:23">
@@ -1607,7 +1601,7 @@
         <v>35</v>
       </c>
       <c r="G15" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:23">
@@ -1630,7 +1624,7 @@
         <v>35</v>
       </c>
       <c r="G16" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:23">
@@ -1653,7 +1647,7 @@
         <v>35</v>
       </c>
       <c r="G17" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:23">
@@ -1676,7 +1670,7 @@
         <v>35</v>
       </c>
       <c r="G18" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:23">
@@ -1699,7 +1693,7 @@
         <v>35</v>
       </c>
       <c r="G19" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:23" s="2" customFormat="1">
@@ -1727,7 +1721,7 @@
         <v>44</v>
       </c>
       <c r="G21" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="U21" t="s">
         <v>45</v>
@@ -1753,7 +1747,7 @@
         <v>49</v>
       </c>
       <c r="G22" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" spans="1:23">
@@ -1776,7 +1770,7 @@
         <v>44</v>
       </c>
       <c r="G23" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="U23" t="s">
         <v>45</v>
@@ -1807,7 +1801,7 @@
         <v>54</v>
       </c>
       <c r="G25" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="W25" t="s">
         <v>55</v>
@@ -1838,7 +1832,7 @@
         <v>60</v>
       </c>
       <c r="G27" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="28" spans="1:23">
@@ -1861,7 +1855,7 @@
         <v>87</v>
       </c>
       <c r="G28" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="I28" t="s">
         <v>88</v>
@@ -1902,7 +1896,7 @@
         <v>97</v>
       </c>
       <c r="G29" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="I29" t="s">
         <v>88</v>
@@ -1943,7 +1937,7 @@
         <v>105</v>
       </c>
       <c r="G30" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="I30" t="s">
         <v>88</v>
@@ -1984,7 +1978,7 @@
         <v>113</v>
       </c>
       <c r="G31" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:23">
@@ -2007,7 +2001,7 @@
         <v>118</v>
       </c>
       <c r="G32" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="33" spans="1:22">
@@ -2030,7 +2024,7 @@
         <v>122</v>
       </c>
       <c r="G33" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:22">
@@ -2088,7 +2082,7 @@
         <v>305010013</v>
       </c>
       <c r="G35" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="P35" t="s">
         <v>129</v>
@@ -2102,7 +2096,7 @@
         <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C36" t="s">
         <v>134</v>
@@ -2117,7 +2111,7 @@
         <v>137</v>
       </c>
       <c r="G36" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:22" s="2" customFormat="1">
@@ -2130,10 +2124,10 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C38" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" spans="1:22">
@@ -2141,13 +2135,13 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C39" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D39" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E39" t="s">
         <v>140</v>
@@ -2173,7 +2167,7 @@
         <v>139</v>
       </c>
       <c r="G40" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="41" spans="1:22">
@@ -2193,7 +2187,7 @@
         <v>142</v>
       </c>
       <c r="G41" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" spans="1:22">
@@ -2233,7 +2227,7 @@
         <v>159</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:22">
@@ -2253,7 +2247,7 @@
         <v>23</v>
       </c>
       <c r="G44" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:22">
@@ -2270,7 +2264,7 @@
         <v>22</v>
       </c>
       <c r="G45" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="46" spans="1:22">
@@ -2287,7 +2281,7 @@
         <v>61</v>
       </c>
       <c r="F46" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="47" spans="1:22">
@@ -2298,7 +2292,7 @@
         <v>164</v>
       </c>
       <c r="F47" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="48" spans="1:22">

</xml_diff>